<commit_message>
Change CF to zero
Make zero the CF of "Water, unspecified natural origin" in	"natural resource::in water"
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\bw_methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F67392-7745-478E-9C48-6D94B190E05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F2A94D-BA19-4067-884C-3893680B5214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-15000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,7 +522,7 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Make CF of "Water, unspecified natural origin" (natural resource::fossil well) = 1E-9
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F2A94D-BA19-4067-884C-3893680B5214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44A49CB-37F9-4097-AA29-CD55A50EC67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-15000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +533,7 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Make CF of "Water, unspecified natural origin"(natural resource::in ground) = 1E-9
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44A49CB-37F9-4097-AA29-CD55A50EC67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5D96F5-7398-4663-9107-9F36F007A6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-15000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60120" yWindow="-22170" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +533,7 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -544,7 +544,7 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Make CF of "Water, turbine use, unspecified natural origin" (natural resource::in water) = 1E-9
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5D96F5-7398-4663-9107-9F36F007A6AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476243AE-0A0D-4D4D-9E4D-1C142C1E1822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60120" yWindow="-22170" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-15000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +511,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -544,7 +544,7 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Make CF of "Water, cooling, unspecified natural origin" (natural resource::in water) = 1E-9
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476243AE-0A0D-4D4D-9E4D-1C142C1E1822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2679672-620B-477B-A4A7-7A855D672664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-15000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -456,7 +456,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -511,7 +511,7 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>1.0000000000000001E-9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add "unspecified natural origin" CFs for FWU PB
- "Water, unspecified natural origin" (natural resource::fossil well)
- "Water, unspecified natural origin" (natural resource::in ground)
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\bw_methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F67392-7745-478E-9C48-6D94B190E05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9145D356-D4FF-4338-A27D-51548106E66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8400" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-15000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
+      <selection activeCell="A11" sqref="A11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,7 +533,7 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -544,7 +544,7 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add CFs for FWU PB
- "Water, cooling, unspecified natural origin" (natural resource::in water) = 1E-9
- "Water, turbine use, unspecified natural origin" (natural resource::in water) = 1E-9
- "Water" (water) = -1E-9

These three flows should "mostly" cancel each other
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9145D356-D4FF-4338-A27D-51548106E66D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782E109B-EEFE-4736-9317-B790F6C83110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-15000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>natural resource::in ground</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
 </sst>
 </file>
@@ -99,12 +102,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,9 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -455,8 +472,8 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="C4" s="3">
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -510,8 +527,8 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9">
-        <v>0</v>
+      <c r="C9" s="3">
+        <v>1.0000000000000001E-9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -532,7 +549,7 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
@@ -543,7 +560,7 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
@@ -556,6 +573,17 @@
       </c>
       <c r="C13">
         <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-1.0000000000000001E-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove CF (make FWU PB as in simapro)
Set to zero:
- "Water, unspecified natural origin" (natural resource::in water)

With this change the results for FWU PB in bw and in simapro are "practically" identical.
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F2A94D-BA19-4067-884C-3893680B5214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1C6491-F5D8-4A8B-95A2-ACF7BB9378FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-15000" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,12 +99,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -119,9 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +412,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,13 +522,13 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make FWU PB as in simapro
cherrypicked from d38cf18f81a83b6
</commit_message>
<xml_diff>
--- a/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
+++ b/src/aesa_pbs/data/aesa_FreshwaterUse_Global.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ViteksPC\Documents\00-ETH_projects\AESAmethods\src\aesa_pbs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608EDBC5-A6F8-4494-A926-054DD1FDF18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1C6491-F5D8-4A8B-95A2-ACF7BB9378FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -76,15 +76,6 @@
   </si>
   <si>
     <t>natural resource::in ground</t>
-  </si>
-  <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>water::fossil well</t>
-  </si>
-  <si>
-    <t>water::ground-, long-term</t>
   </si>
 </sst>
 </file>
@@ -108,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,12 +109,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -140,11 +125,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -478,8 +462,8 @@
       <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="3">
-        <v>1.0000000000000001E-9</v>
+      <c r="C4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -533,19 +517,19 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3">
-        <v>1.0000000000000001E-9</v>
+      <c r="C9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>1.0000000000000001E-9</v>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -555,8 +539,8 @@
       <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="2">
-        <v>1.0000000000000001E-9</v>
+      <c r="C11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -566,8 +550,8 @@
       <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="2">
-        <v>1.0000000000000001E-9</v>
+      <c r="C12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -579,39 +563,6 @@
       </c>
       <c r="C13">
         <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="3">
-        <v>-1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="3">
-        <v>-1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="3">
-        <v>-1.0000000000000001E-9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>